<commit_message>
add excel file to manage posters
</commit_message>
<xml_diff>
--- a/new/docs/posters.xlsx
+++ b/new/docs/posters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>شماره پوستر</t>
   </si>
@@ -39,6 +39,294 @@
   </si>
   <si>
     <t>رسیده/نرسیده</t>
+  </si>
+  <si>
+    <t>Casimir force between topological insulators</t>
+  </si>
+  <si>
+    <t>Allameh, Nazanin; Tajik, Fatemeh; Masoudi, Amirali</t>
+  </si>
+  <si>
+    <t>Shirvani , Fatemeh; Shokri, Aliasghar; Abedi Ravan, Bahram</t>
+  </si>
+  <si>
+    <t>Tunability of defect mode based on magnetized two-dimensional plasma photonic crystal</t>
+  </si>
+  <si>
+    <t>Karami Garehgeshlagi, Fahimeh; Jamshidi, Kazem;</t>
+  </si>
+  <si>
+    <r>
+      <t>Studying of electronic properties of monolayer Ti</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Zr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1-x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N alloy using first principle calculation of quantum mechanic</t>
+    </r>
+  </si>
+  <si>
+    <t>Pourfarrokh Navidehi, Mojtaba; Bagheri Tajani, Meysam</t>
+  </si>
+  <si>
+    <t>Experimental study of liposome aggregation</t>
+  </si>
+  <si>
+    <t>Jamali, Ramin; Moradi, Ali-Reza</t>
+  </si>
+  <si>
+    <t>Investigating the time evolution of color distribution in a variety of surfaces</t>
+  </si>
+  <si>
+    <t>Jamali, Ramin; Ohadi, Taha; Moradi, Ali-Reza</t>
+  </si>
+  <si>
+    <t>Layer Dependence of Thermal Conductivity of Zigzag and Armchair Graphene Nanoribbons</t>
+  </si>
+  <si>
+    <t>Mehri, Ali; Jamaati, Maryam; Pahlavan Yali, Reza</t>
+  </si>
+  <si>
+    <r>
+      <t>Comparison of magnetic order in single layer CrTe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> in T and H phases</t>
+    </r>
+  </si>
+  <si>
+    <t>The Effect of Zinc Compounds on Toxicity and Stbility of Organo-Metal Halide Perovskite Materials</t>
+  </si>
+  <si>
+    <t>Soleimanioun, Nazilla; Mukul, Monika; Sharma, Sameeksha; Rani, Mamta; Tripathi S.K.</t>
+  </si>
+  <si>
+    <t>Spin-orbit coupling effects on transport properties of electronic Lieb lattice in the presence of magnetic field</t>
+  </si>
+  <si>
+    <t>Rezania, Hamed; Sadeghi KHomartaji, Elham</t>
+  </si>
+  <si>
+    <t>Pakmehr, Mehdi; Dehghani, Parnian</t>
+  </si>
+  <si>
+    <t>Dynamics of Rydberg-dressed bosons in a bilayer structure</t>
+  </si>
+  <si>
+    <t>Pouresmaeeli, Fatemeh; Abedinpour, Saeed. H; Tanatar, B.</t>
+  </si>
+  <si>
+    <t>Foadian, Amir; Adelifard, Mehdi</t>
+  </si>
+  <si>
+    <t>Interaction force between two red blood cells in the presence of acoustic waves</t>
+  </si>
+  <si>
+    <t>Eslami, Fateme; Hamzehpour, Hossein; Bahrani, Seyed Amir</t>
+  </si>
+  <si>
+    <t>Hosseini, Seyd Reza; Nahal, Arashmid; Mahjour-Shafiei, Masoud</t>
+  </si>
+  <si>
+    <r>
+      <t>Synthesis and preliminary study of Diluted magnetic Molybdenite (MoS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) in bulk morphology</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>An investigation on the effect of changing sulfur ratio and annealing on the physical properties of Cu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ZnSnS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> thin film</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Index of refraction patterning in ion-exchanged glasses with He</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> Ion-beam</t>
+    </r>
+  </si>
+  <si>
+    <t>Theoretical Study of RNA Polymerase Behavior Against Transcriptional Barriers</t>
+  </si>
+  <si>
+    <t>Kor, Razieh; Mohammad-Rafiee, Farshid</t>
+  </si>
+  <si>
+    <t>Enhancing synchronization in the small-world networks by frustration</t>
+  </si>
+  <si>
+    <t>Mahdavi, Esmaeil; Zarei, Mina; Shahbazi, Farhad</t>
+  </si>
+  <si>
+    <t>Investigation of the effect of nanochannel wall geometry on water flow by molecular dynamics method</t>
+  </si>
+  <si>
+    <t>Torkaman, Mehran; Hamzehpour, Hossein; Manzoor, Kazem; Sarabadani, Jalal</t>
+  </si>
+  <si>
+    <t>Jafari Tilehnoei, Mahdi; Milani Moghaddam, Hossain</t>
+  </si>
+  <si>
+    <r>
+      <t>The effect of the calcination temperature and mole percent on the real and imaginary parts of the dielectric function of TiO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/WO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8.8000000000000007"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> nanoparticles synthesized by the sol-gel method</t>
+    </r>
+  </si>
+  <si>
+    <t>Semi-flexible Polymer Ejection from Spherical Nano-structure</t>
+  </si>
+  <si>
+    <t>Moazemi, Farzaneh; Nikoofard, Narges</t>
   </si>
 </sst>
 </file>
@@ -48,10 +336,34 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-3000401]0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8.8000000000000007"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,12 +389,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,15 +682,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="3" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="207.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -394,283 +714,501 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
         <v>5</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
         <v>6</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
         <v>7</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+      <c r="D12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
         <v>8</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
         <v>9</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
         <v>10</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
         <v>11</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="D16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
         <v>12</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="D17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
         <v>13</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
         <v>14</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+      <c r="D19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
         <v>15</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
         <v>16</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B22" s="3">
         <v>17</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+      <c r="D22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>18</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B25" s="3">
         <v>20</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
+      <c r="D25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
         <v>21</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
         <v>22</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
+      <c r="D27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
         <v>23</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
         <v>24</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="2">
+      <c r="D29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
         <v>25</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
         <v>26</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
         <v>27</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
         <v>28</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
         <v>29</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
         <v>30</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="3">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B36" s="3">
         <v>31</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="3">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
+      <c r="D36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
         <v>32</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="2">
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B38" s="3">
         <v>33</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="2">
+      <c r="D38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
         <v>34</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="3">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="2">
-        <v>35</v>
-      </c>
+      <c r="D39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
     </row>
   </sheetData>
+  <sortState ref="B6:F39">
+    <sortCondition ref="B6:B39"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>